<commit_message>
updated actual sprint burndown chart and added my code review
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/Sprint_Burndown_4.xlsx
+++ b/teamOverview/sprintBacklog/Sprint_Burndown_4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\OneDrive\Documents\ComSci\Year 3 Sem 1\cscc01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/392e16b045ef5b88/Documents/ComSci/Year 3 Sem 1/cscc01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BD4F281F-FE4F-45AD-BC7A-405C1C6D95D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0E450E92-AAD5-4DBE-AD63-80C0DD8C93C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Provisional</t>
   </si>
@@ -471,19 +471,19 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -618,8 +618,8 @@
         <c:axId val="442376048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="43"/>
-          <c:min val="-5"/>
+          <c:max val="30"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1657,10 +1657,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1BB781-C491-4243-859C-AAD93AE5F06E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2130,24 +2130,24 @@
         <v>29</v>
       </c>
       <c r="D15" s="1">
-        <f>C15-SUM(K25:K30)</f>
-        <v>29</v>
+        <f>C15-SUM(K25:K37)</f>
+        <v>27</v>
       </c>
       <c r="E15" s="1">
-        <f>D15-SUM(L25:L30)</f>
-        <v>29</v>
+        <f t="shared" ref="E15:H15" si="2">D15-SUM(L25:L37)</f>
+        <v>27</v>
       </c>
       <c r="F15" s="1">
-        <f>E15-SUM(M25:M30)</f>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="G15" s="1">
-        <f>F15-SUM(N25:N30)</f>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="H15" s="1">
-        <f>G15-SUM(O25:O30)</f>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
@@ -2260,22 +2260,118 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J25" s="1">
+        <v>10</v>
+      </c>
+      <c r="O25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J26" s="1">
+        <v>20</v>
+      </c>
+      <c r="M26" s="1">
+        <v>3</v>
+      </c>
+    </row>
     <row r="27" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="1">
+        <v>21</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="4"/>
+    </row>
+    <row r="28" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M28" s="1">
         <v>3</v>
       </c>
-      <c r="Q27" s="4"/>
+    </row>
+    <row r="29" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O29" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J30" s="1">
+        <v>25</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J31" s="1" t="s">
+      <c r="J31" s="1">
+        <v>26</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J32" s="1">
+        <v>27</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="J33" s="1">
+        <v>28</v>
+      </c>
+      <c r="M33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="J34" s="1">
+        <v>29</v>
+      </c>
+      <c r="M34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="J35" s="1">
+        <v>30</v>
+      </c>
+      <c r="M35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="J36" s="1">
+        <v>31</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="J37" s="1">
+        <v>32</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="J38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K31" s="1">
-        <f>SUM(K25:O30)</f>
-        <v>3</v>
+      <c r="K38" s="1">
+        <f>SUM(K25:O37)</f>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>